<commit_message>
další pokrok v barikádnících
</commit_message>
<xml_diff>
--- a/longitude - latitude/barikadnici-toponyma.xlsx
+++ b/longitude - latitude/barikadnici-toponyma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\korpus_prozy\korpusprozy\longitude - latitude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9815D9E0-D91D-4E5A-A80B-B05F742F9EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE24DCFA-CE49-4AA8-AF27-1B609DBAD6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="552" yWindow="888" windowWidth="7548" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="156">
   <si>
     <t>longitude</t>
   </si>
@@ -37,9 +37,6 @@
     <t>náměstí Marianské</t>
   </si>
   <si>
-    <t>Svornosti</t>
-  </si>
-  <si>
     <t>Hradčany</t>
   </si>
   <si>
@@ -257,12 +254,6 @@
   </si>
   <si>
     <t>14.417541904255318</t>
-  </si>
-  <si>
-    <t>50.0695011</t>
-  </si>
-  <si>
-    <t>14.4091264</t>
   </si>
   <si>
     <t>50.0687486</t>
@@ -859,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -877,7 +868,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -886,12 +877,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -900,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -908,24 +899,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -933,10 +924,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -944,26 +935,29 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -972,12 +966,12 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -986,21 +980,18 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>65</v>
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1008,26 +999,26 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>86</v>
@@ -1035,19 +1026,22 @@
       <c r="C14" t="s">
         <v>85</v>
       </c>
+      <c r="D14" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" t="s">
-        <v>88</v>
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1061,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1075,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1089,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1103,12 +1097,12 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1117,98 +1111,98 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>65</v>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" t="s">
-        <v>91</v>
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>65</v>
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" t="s">
-        <v>93</v>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" t="s">
-        <v>68</v>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
         <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1217,92 +1211,92 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>65</v>
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
         <v>96</v>
-      </c>
-      <c r="C30" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" t="s">
-        <v>99</v>
+        <v>17</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32" t="s">
-        <v>65</v>
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" t="s">
-        <v>101</v>
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34" t="s">
-        <v>65</v>
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
         <v>104</v>
       </c>
       <c r="C35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1311,38 +1305,35 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
         <v>105</v>
-      </c>
-      <c r="D36" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B37" t="s">
-        <v>109</v>
-      </c>
-      <c r="C37" t="s">
-        <v>108</v>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38" t="s">
-        <v>65</v>
+      <c r="B38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1350,10 +1341,10 @@
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1361,10 +1352,10 @@
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1372,21 +1363,21 @@
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1394,26 +1385,26 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
         <v>123</v>
@@ -1421,58 +1412,58 @@
       <c r="C45" t="s">
         <v>122</v>
       </c>
+      <c r="D45" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" t="s">
-        <v>125</v>
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47" t="s">
-        <v>65</v>
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B48" t="s">
-        <v>128</v>
-      </c>
-      <c r="C48" t="s">
-        <v>127</v>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49" t="s">
-        <v>65</v>
+      <c r="B49" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1480,10 +1471,13 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="D50" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1491,52 +1485,49 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>131</v>
-      </c>
-      <c r="D51" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
         <v>134</v>
       </c>
       <c r="C52" t="s">
         <v>133</v>
+      </c>
+      <c r="D52" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B53" t="s">
-        <v>137</v>
-      </c>
-      <c r="C53" t="s">
-        <v>136</v>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54" t="s">
         <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1544,10 +1535,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1555,10 +1546,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1566,60 +1557,63 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
-        <v>145</v>
-      </c>
-      <c r="C58" t="s">
-        <v>144</v>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-      <c r="D59" t="s">
-        <v>65</v>
+      <c r="B59" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
         <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>147</v>
-      </c>
-      <c r="C60" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" t="s">
+        <v>145</v>
       </c>
       <c r="D61" t="s">
-        <v>60</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1641,10 +1635,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" t="s">
         <v>152</v>
-      </c>
-      <c r="C63" t="s">
-        <v>151</v>
       </c>
       <c r="D63" t="s">
         <v>153</v>
@@ -1655,24 +1649,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" t="s">
         <v>154</v>
-      </c>
-      <c r="C64" t="s">
-        <v>155</v>
-      </c>
-      <c r="D64" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>158</v>
-      </c>
-      <c r="C65" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
další progres v barikádnících mimochodem - všechno nejlepší k svátku, pane docente!
</commit_message>
<xml_diff>
--- a/longitude - latitude/barikadnici-toponyma.xlsx
+++ b/longitude - latitude/barikadnici-toponyma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\korpus_prozy\korpusprozy\longitude - latitude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A36E60E-42E9-4485-8EC7-345D914E9A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75023E5-6657-43E6-8CC0-1E1B0E529D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="444" windowWidth="7548" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="444" windowWidth="7548" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
dokončeni barikádníci (až na pár otazníků)
</commit_message>
<xml_diff>
--- a/longitude - latitude/barikadnici-toponyma.xlsx
+++ b/longitude - latitude/barikadnici-toponyma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\korpus_prozy\korpusprozy\longitude - latitude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75023E5-6657-43E6-8CC0-1E1B0E529D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2FAE76-D28C-482D-8412-5CB2F043FCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="444" windowWidth="7548" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -856,7 +856,7 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>